<commit_message>
Subindo tudo para o GitHub
</commit_message>
<xml_diff>
--- a/Base/Backlog_13.xlsx
+++ b/Base/Backlog_13.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franciscoj\Python_Initial\Pyhton_Web\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1AD9CB-7F77-43EE-B0BC-DE2BF244547C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE8E110-EDEA-4E1E-87A6-85A919E7741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="418" activeTab="1" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
   </bookViews>
@@ -109,10 +109,10 @@
     <t>Higor Cruz</t>
   </si>
   <si>
-    <t>Mara neves</t>
-  </si>
-  <si>
     <t>Resolvido</t>
+  </si>
+  <si>
+    <t>Mara Neves</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6">
         <v>2025</v>
@@ -647,7 +647,7 @@
         <v>45747</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>15</v>
@@ -682,7 +682,7 @@
         <v>45747</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>15</v>
@@ -717,7 +717,7 @@
         <v>45747</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>15</v>
@@ -752,7 +752,7 @@
         <v>45747</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>15</v>
@@ -862,10 +862,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -920,7 +921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
@@ -949,13 +950,13 @@
         <v>45747</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -984,13 +985,13 @@
         <v>45747</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
@@ -1124,13 +1125,13 @@
         <v>45747</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
@@ -1159,13 +1160,13 @@
         <v>45747</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>4</v>
       </c>
@@ -1194,7 +1195,7 @@
         <v>45747</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" s="15" t="s">
         <v>11</v>
@@ -1235,7 +1236,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>4</v>
       </c>
@@ -1264,13 +1265,13 @@
         <v>45747</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -1281,7 +1282,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
@@ -1292,7 +1293,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
@@ -1303,7 +1304,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
@@ -1314,7 +1315,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
@@ -1649,6 +1650,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J16" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}">
+    <filterColumn colId="7">
+      <filters>
+        <dateGroupItem year="2025" month="3" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Pendente"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J16">
       <sortCondition ref="B1:B16"/>
     </sortState>

</xml_diff>